<commit_message>
0.005 - Added schematic page with fully working search
</commit_message>
<xml_diff>
--- a/data/schematics.xlsx
+++ b/data/schematics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\4uck0ff.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B38E17-60C8-4323-8ECF-169317959D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D87223B-B5EE-42BE-AA46-4AC086FC0D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="78">
   <si>
     <t>Описание</t>
   </si>
@@ -109,6 +109,156 @@
   </si>
   <si>
     <t>20.20.2055</t>
+  </si>
+  <si>
+    <t>888A</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>1234G</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>Lada</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Geely</t>
+  </si>
+  <si>
+    <t>20.20.2056</t>
+  </si>
+  <si>
+    <t>20.20.2057</t>
+  </si>
+  <si>
+    <t>20.20.2058</t>
+  </si>
+  <si>
+    <t>20.20.2059</t>
+  </si>
+  <si>
+    <t>20.20.2060</t>
+  </si>
+  <si>
+    <t>20.20.2061</t>
+  </si>
+  <si>
+    <t>20.20.2062</t>
+  </si>
+  <si>
+    <t>20.20.2063</t>
+  </si>
+  <si>
+    <t>20.20.2064</t>
+  </si>
+  <si>
+    <t>20.20.2065</t>
+  </si>
+  <si>
+    <t>20.20.2066</t>
+  </si>
+  <si>
+    <t>20.20.2067</t>
+  </si>
+  <si>
+    <t>20.20.2068</t>
+  </si>
+  <si>
+    <t>20.20.2069</t>
+  </si>
+  <si>
+    <t>20.20.2070</t>
+  </si>
+  <si>
+    <t>20.20.2071</t>
+  </si>
+  <si>
+    <t>20.20.2072</t>
+  </si>
+  <si>
+    <t>20.20.2073</t>
+  </si>
+  <si>
+    <t>20.20.2074</t>
+  </si>
+  <si>
+    <t>Vesta</t>
+  </si>
+  <si>
+    <t>Lancer</t>
+  </si>
+  <si>
+    <t>E50</t>
+  </si>
+  <si>
+    <t>Escort</t>
+  </si>
+  <si>
+    <t>X50</t>
+  </si>
+  <si>
+    <t>E38</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>E34</t>
+  </si>
+  <si>
+    <t>Polo</t>
+  </si>
+  <si>
+    <t>X70</t>
+  </si>
+  <si>
+    <t>Largus</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Kadjar</t>
+  </si>
+  <si>
+    <t>Maybach</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>Jetta</t>
+  </si>
+  <si>
+    <t>Qashqai</t>
+  </si>
+  <si>
+    <t>Corolla</t>
+  </si>
+  <si>
+    <t>C63</t>
   </si>
 </sst>
 </file>
@@ -446,17 +596,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" customWidth="1"/>
@@ -478,8 +629,8 @@
       <c r="D1">
         <v>1998</v>
       </c>
-      <c r="E1">
-        <v>888</v>
+      <c r="E1" t="s">
+        <v>28</v>
       </c>
       <c r="F1">
         <v>26677</v>
@@ -516,8 +667,8 @@
       <c r="D2">
         <v>1999</v>
       </c>
-      <c r="E2" s="3">
-        <v>777777777</v>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F2">
         <v>26678</v>
@@ -554,8 +705,8 @@
       <c r="D3">
         <v>2005</v>
       </c>
-      <c r="E3" s="3">
-        <v>123456789</v>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F3">
         <v>26679</v>
@@ -587,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="D4">
         <v>1998</v>
@@ -622,16 +773,16 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="D5">
         <v>1998</v>
       </c>
-      <c r="E5">
-        <v>888</v>
+      <c r="E5" t="s">
+        <v>28</v>
       </c>
       <c r="F5">
         <v>26681</v>
@@ -660,16 +811,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>1999</v>
       </c>
-      <c r="E6" s="3">
-        <v>777777777</v>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F6">
         <v>26682</v>
@@ -698,7 +849,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -706,8 +857,8 @@
       <c r="D7">
         <v>2005</v>
       </c>
-      <c r="E7" s="3">
-        <v>123456789</v>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F7">
         <v>26683</v>
@@ -736,10 +887,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <v>1998</v>
@@ -774,16 +925,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D9">
-        <v>1998</v>
-      </c>
-      <c r="E9">
-        <v>888</v>
+        <v>1997</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
       </c>
       <c r="F9">
         <v>26685</v>
@@ -812,16 +963,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>1999</v>
       </c>
-      <c r="E10" s="3">
-        <v>777777777</v>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F10">
         <v>26686</v>
@@ -850,16 +1001,16 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D11">
         <v>2005</v>
       </c>
-      <c r="E11" s="3">
-        <v>123456789</v>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F11">
         <v>26687</v>
@@ -888,10 +1039,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>2005</v>
@@ -918,6 +1069,728 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>1998</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>26689</v>
+      </c>
+      <c r="G13">
+        <v>11.09</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14">
+        <v>1999</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>26690</v>
+      </c>
+      <c r="G14">
+        <v>11.59</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>2005</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <v>26691</v>
+      </c>
+      <c r="G15">
+        <v>12.09</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16">
+        <v>1998</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>26692</v>
+      </c>
+      <c r="G16">
+        <v>12.59</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <v>1998</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17">
+        <v>26693</v>
+      </c>
+      <c r="G17">
+        <v>13.09</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18">
+        <v>1999</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18">
+        <v>26694</v>
+      </c>
+      <c r="G18">
+        <v>13.59</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>2005</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>26695</v>
+      </c>
+      <c r="G19">
+        <v>14.09</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20">
+        <v>1998</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>26696</v>
+      </c>
+      <c r="G20">
+        <v>14.59</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21">
+        <v>1998</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21">
+        <v>26697</v>
+      </c>
+      <c r="G21">
+        <v>15.09</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22">
+        <v>1999</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22">
+        <v>26698</v>
+      </c>
+      <c r="G22">
+        <v>15.59</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>2005</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>26699</v>
+      </c>
+      <c r="G23">
+        <v>16.09</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24">
+        <v>2005</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>26700</v>
+      </c>
+      <c r="G24">
+        <v>16.59</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>1997</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>26701</v>
+      </c>
+      <c r="G25">
+        <v>17.09</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>2003</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26">
+        <v>26702</v>
+      </c>
+      <c r="G26">
+        <v>17.59</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>2015</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <v>26703</v>
+      </c>
+      <c r="G27">
+        <v>18.09</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>2001</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>26704</v>
+      </c>
+      <c r="G28">
+        <v>18.59</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29">
+        <v>2022</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>26705</v>
+      </c>
+      <c r="G29">
+        <v>19.09</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>2018</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <v>26706</v>
+      </c>
+      <c r="G30">
+        <v>19.59</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31">
+        <v>1995</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>26707</v>
+      </c>
+      <c r="G31">
+        <v>20.09</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
         <v>0</v>
       </c>
     </row>
@@ -960,6 +1833,63 @@
     <hyperlink ref="I10" r:id="rId34" xr:uid="{06F54870-F6C8-41F2-B2C9-7E31B2432EE9}"/>
     <hyperlink ref="J10" r:id="rId35" xr:uid="{CDA552ED-893B-487C-8C32-7042E65F0E11}"/>
     <hyperlink ref="K10" r:id="rId36" xr:uid="{4ECD8916-1BD9-4FE5-B711-6C6CEA89223A}"/>
+    <hyperlink ref="I15" r:id="rId37" xr:uid="{8730E02B-8DC9-4282-9433-F653E65B5567}"/>
+    <hyperlink ref="I27" r:id="rId38" xr:uid="{3E86747B-8D14-4EE2-AB70-7B9FDE32F53F}"/>
+    <hyperlink ref="J15" r:id="rId39" xr:uid="{7D7B3BAF-5F3B-4F48-B151-EFCA260AFCE0}"/>
+    <hyperlink ref="J27" r:id="rId40" xr:uid="{DDE716D1-8630-4A93-B0F1-F6E48E4C8995}"/>
+    <hyperlink ref="K15" r:id="rId41" xr:uid="{37A47411-1DE1-4075-9CBC-0DD45D30C7E1}"/>
+    <hyperlink ref="K27" r:id="rId42" xr:uid="{80E29C77-031B-4A0A-8D3B-64F9FD391D39}"/>
+    <hyperlink ref="I16" r:id="rId43" xr:uid="{8201C7D6-EFF6-4429-92EC-AE2B16BEBBA8}"/>
+    <hyperlink ref="I28" r:id="rId44" xr:uid="{E9DB0274-E12A-40C0-A122-251EF3788BF4}"/>
+    <hyperlink ref="J16" r:id="rId45" xr:uid="{F52405BE-751A-4AF0-8A48-C3A1F6883255}"/>
+    <hyperlink ref="J28" r:id="rId46" xr:uid="{92D98417-4E2A-4024-A936-4F4E73C05870}"/>
+    <hyperlink ref="K16" r:id="rId47" xr:uid="{0DB73916-8847-4692-87B6-0C8D2A1B1BE6}"/>
+    <hyperlink ref="K28" r:id="rId48" xr:uid="{88507BE5-E786-4B4B-9AD3-A9376233558C}"/>
+    <hyperlink ref="I13" r:id="rId49" xr:uid="{BB4170CB-5503-4E97-AD17-6248D6CC60E7}"/>
+    <hyperlink ref="I25" r:id="rId50" xr:uid="{AEB86730-089B-48E4-93FF-3AD3B650E630}"/>
+    <hyperlink ref="J13" r:id="rId51" xr:uid="{5C232115-65A3-4D1A-9C6D-1A90688A9A98}"/>
+    <hyperlink ref="J25" r:id="rId52" xr:uid="{5E4B9F5C-DBB0-427D-8796-26C3D28F555C}"/>
+    <hyperlink ref="K13" r:id="rId53" xr:uid="{FFC1E05D-BB24-4C79-A2DA-93CA4DD3FF27}"/>
+    <hyperlink ref="K25" r:id="rId54" xr:uid="{714533E3-00BA-4FB3-9136-DEB50A2A0BBC}"/>
+    <hyperlink ref="I14" r:id="rId55" xr:uid="{6C55B1C8-85F2-4DA3-B685-67EAD2061534}"/>
+    <hyperlink ref="I26" r:id="rId56" xr:uid="{731AE77D-5084-4695-B024-1231B155EFB5}"/>
+    <hyperlink ref="J14" r:id="rId57" xr:uid="{0A54B13B-6E5A-455D-AAD2-454AA5A15DD1}"/>
+    <hyperlink ref="J26" r:id="rId58" xr:uid="{8C3B611D-DBC0-4EB4-9957-4B2B92D01DF3}"/>
+    <hyperlink ref="K14" r:id="rId59" xr:uid="{DB3B7431-58EC-497F-9B0F-B31AB805A672}"/>
+    <hyperlink ref="K26" r:id="rId60" xr:uid="{3CB7236A-D211-4BCA-851E-7FF9E4E6BEAC}"/>
+    <hyperlink ref="I19" r:id="rId61" xr:uid="{CA98193C-4EA4-45B6-9934-01015C3B5298}"/>
+    <hyperlink ref="I31" r:id="rId62" xr:uid="{FA08D932-72AF-4821-A1ED-F3A0119EF632}"/>
+    <hyperlink ref="J19" r:id="rId63" xr:uid="{36585E95-EF8F-4CD9-B099-ED4162489F92}"/>
+    <hyperlink ref="J31" r:id="rId64" xr:uid="{940FA059-7E88-4F7A-925F-D10DC50DC6E7}"/>
+    <hyperlink ref="K19" r:id="rId65" xr:uid="{E7BED3D2-3336-455B-9E9E-D4BA73E156A4}"/>
+    <hyperlink ref="K31" r:id="rId66" xr:uid="{817DC0E9-9E98-4C3F-A1BE-C5CA71D79BB1}"/>
+    <hyperlink ref="I20" r:id="rId67" xr:uid="{81081C4F-C0D0-467F-BAB0-9551B7BBF235}"/>
+    <hyperlink ref="J20" r:id="rId68" xr:uid="{D587259B-1139-46F6-8DC9-EEEEFA335C68}"/>
+    <hyperlink ref="K20" r:id="rId69" xr:uid="{458ED017-181C-4F12-8802-F00EF64793D9}"/>
+    <hyperlink ref="I17" r:id="rId70" xr:uid="{B34342A1-92E7-4FDB-98D4-6AFC3F37C896}"/>
+    <hyperlink ref="I29" r:id="rId71" xr:uid="{F3D34B90-686E-4F35-99B6-8C7E78453F88}"/>
+    <hyperlink ref="J17" r:id="rId72" xr:uid="{CA269FA9-B0B5-4307-B498-257C00727711}"/>
+    <hyperlink ref="J29" r:id="rId73" xr:uid="{1353AA98-36B0-48E1-AACB-E8FAB9BC11D6}"/>
+    <hyperlink ref="K17" r:id="rId74" xr:uid="{60756446-141F-49AB-9700-FE97D511D3DF}"/>
+    <hyperlink ref="K29" r:id="rId75" xr:uid="{8BE3A974-DE12-4835-BBA7-98A394B2FE11}"/>
+    <hyperlink ref="I18" r:id="rId76" xr:uid="{30014843-15D9-4E2B-807C-3AE0FBA061B4}"/>
+    <hyperlink ref="I30" r:id="rId77" xr:uid="{971A7AD3-B14A-4D12-B557-908CC1BB0A6E}"/>
+    <hyperlink ref="J18" r:id="rId78" xr:uid="{68EF6F0D-8C61-4CD1-A744-C2E6E0335FAB}"/>
+    <hyperlink ref="J30" r:id="rId79" xr:uid="{300339A7-F305-4E68-B7F9-9A2DF49466F7}"/>
+    <hyperlink ref="K18" r:id="rId80" xr:uid="{3DD9A827-88D5-4337-9C7B-6F8D812364C1}"/>
+    <hyperlink ref="K30" r:id="rId81" xr:uid="{E7F379DD-7B50-4AB7-8FD6-7800DC10CB5A}"/>
+    <hyperlink ref="I23" r:id="rId82" xr:uid="{C7A96136-11A2-4DEC-8B72-C6535A6F3081}"/>
+    <hyperlink ref="J23" r:id="rId83" xr:uid="{2CFA4DDF-71DC-4108-BEB1-9BAAFD396EF5}"/>
+    <hyperlink ref="K23" r:id="rId84" xr:uid="{BCFB2B88-E7E9-421A-8996-4DFAA91D2AA3}"/>
+    <hyperlink ref="I24" r:id="rId85" xr:uid="{4AE1BA04-F77F-4E3E-81F2-4177C85B81AE}"/>
+    <hyperlink ref="J24" r:id="rId86" xr:uid="{8F879E24-70BD-4836-A62D-7C125C06CE5E}"/>
+    <hyperlink ref="K24" r:id="rId87" xr:uid="{2172D550-E2DE-4F65-85B4-80D8C1E774D7}"/>
+    <hyperlink ref="I21" r:id="rId88" xr:uid="{996D5064-F030-4D58-951D-CCA7BB9963FC}"/>
+    <hyperlink ref="J21" r:id="rId89" xr:uid="{8EC19C25-A430-4580-8CE2-256703DD9F5C}"/>
+    <hyperlink ref="K21" r:id="rId90" xr:uid="{416F7B63-AD62-4B5A-9A6F-14B9BCA5E6B7}"/>
+    <hyperlink ref="I22" r:id="rId91" xr:uid="{1DEBF2A9-D072-4755-8061-D7A06016E285}"/>
+    <hyperlink ref="J22" r:id="rId92" xr:uid="{A858FE99-2F64-4043-911B-6C336FD8967E}"/>
+    <hyperlink ref="K22" r:id="rId93" xr:uid="{0F45A4F5-2732-4422-A7DD-EAEB1BA786FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>